<commit_message>
Criação dos arquivos .py com cada função, as constantes e funcoes auxiliares
</commit_message>
<xml_diff>
--- a/Dataframe/curva_forward.xlsx
+++ b/Dataframe/curva_forward.xlsx
@@ -163,223 +163,223 @@
     <t>2025-12-09T03:00:00.000Z</t>
   </si>
   <si>
-    <t>2023-01-09T03:00:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.892Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.904Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.911Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.917Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.925Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.932Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.939Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.945Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.952Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.959Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.966Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.973Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.980Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.986Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.992Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:58.999Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.008Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.015Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.022Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.029Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.035Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.043Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.049Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.055Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.062Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.069Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.076Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.083Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.090Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.097Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.104Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.112Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.120Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.128Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.135Z</t>
-  </si>
-  <si>
-    <t>2023-01-10T05:31:59.143Z</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb2</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb3</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb4</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb5</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb6</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb7</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb8</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eb9</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296eba</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ebb</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ebc</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ebd</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ebe</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ebf</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ec0</t>
-  </si>
-  <si>
-    <t>63bcf84e0f9fa90018296ec1</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec2</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec3</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec4</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec5</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec6</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec7</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec8</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ec9</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296eca</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ecb</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ecc</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ecd</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ece</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ecf</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed0</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed1</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed2</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed3</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed4</t>
-  </si>
-  <si>
-    <t>63bcf84f0f9fa90018296ed5</t>
+    <t>2023-01-10T03:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.915Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.926Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.933Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.941Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.948Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.955Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.962Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.969Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.976Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.982Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.989Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:11.997Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.004Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.015Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.022Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.029Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.036Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.043Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.050Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.058Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.065Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.072Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.079Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.086Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.093Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.100Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.107Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.114Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.121Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.129Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.135Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.142Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.148Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.155Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.162Z</t>
+  </si>
+  <si>
+    <t>2023-01-11T05:32:12.169Z</t>
+  </si>
+  <si>
+    <t>63be49dbc72b220018888298</t>
+  </si>
+  <si>
+    <t>63be49dbc72b220018888299</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829a</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829b</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829c</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829d</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829e</t>
+  </si>
+  <si>
+    <t>63be49dbc72b22001888829f</t>
+  </si>
+  <si>
+    <t>63be49dbc72b2200188882a0</t>
+  </si>
+  <si>
+    <t>63be49dbc72b2200188882a1</t>
+  </si>
+  <si>
+    <t>63be49dbc72b2200188882a2</t>
+  </si>
+  <si>
+    <t>63be49dbc72b2200188882a3</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a4</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a5</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a6</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a7</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a8</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882a9</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882aa</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882ab</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882ac</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882ad</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882ae</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882af</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b0</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b1</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b2</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b3</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b4</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b5</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b6</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b7</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b8</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882b9</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882ba</t>
+  </si>
+  <si>
+    <t>63be49dcc72b2200188882bb</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>69.01000000000001</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
@@ -831,7 +831,7 @@
         <v>14</v>
       </c>
       <c r="F3">
-        <v>69.26000000000001</v>
+        <v>69.7</v>
       </c>
       <c r="G3" t="s">
         <v>49</v>
@@ -866,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="F4">
-        <v>69.88</v>
+        <v>69.62</v>
       </c>
       <c r="G4" t="s">
         <v>49</v>
@@ -901,7 +901,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>70.5</v>
+        <v>70.12</v>
       </c>
       <c r="G5" t="s">
         <v>49</v>
@@ -936,7 +936,7 @@
         <v>17</v>
       </c>
       <c r="F6">
-        <v>70.3</v>
+        <v>70.38</v>
       </c>
       <c r="G6" t="s">
         <v>49</v>
@@ -971,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="F7">
-        <v>73</v>
+        <v>72.75</v>
       </c>
       <c r="G7" t="s">
         <v>49</v>
@@ -1006,7 +1006,7 @@
         <v>19</v>
       </c>
       <c r="F8">
-        <v>76.25</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G8" t="s">
         <v>49</v>
@@ -1041,7 +1041,7 @@
         <v>20</v>
       </c>
       <c r="F9">
-        <v>76.25</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G9" t="s">
         <v>49</v>
@@ -1076,7 +1076,7 @@
         <v>21</v>
       </c>
       <c r="F10">
-        <v>76.25</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G10" t="s">
         <v>49</v>
@@ -1111,7 +1111,7 @@
         <v>22</v>
       </c>
       <c r="F11">
-        <v>81</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G11" t="s">
         <v>49</v>
@@ -1146,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="F12">
-        <v>81</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G12" t="s">
         <v>49</v>
@@ -1181,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="F13">
-        <v>81</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="G13" t="s">
         <v>49</v>
@@ -1216,7 +1216,7 @@
         <v>25</v>
       </c>
       <c r="F14">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G14" t="s">
         <v>49</v>
@@ -1251,7 +1251,7 @@
         <v>26</v>
       </c>
       <c r="F15">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G15" t="s">
         <v>49</v>
@@ -1286,7 +1286,7 @@
         <v>27</v>
       </c>
       <c r="F16">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G16" t="s">
         <v>49</v>
@@ -1321,7 +1321,7 @@
         <v>28</v>
       </c>
       <c r="F17">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G17" t="s">
         <v>49</v>
@@ -1356,7 +1356,7 @@
         <v>29</v>
       </c>
       <c r="F18">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G18" t="s">
         <v>49</v>
@@ -1391,7 +1391,7 @@
         <v>30</v>
       </c>
       <c r="F19">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G19" t="s">
         <v>49</v>
@@ -1426,7 +1426,7 @@
         <v>31</v>
       </c>
       <c r="F20">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G20" t="s">
         <v>49</v>
@@ -1461,7 +1461,7 @@
         <v>32</v>
       </c>
       <c r="F21">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G21" t="s">
         <v>49</v>
@@ -1496,7 +1496,7 @@
         <v>33</v>
       </c>
       <c r="F22">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G22" t="s">
         <v>49</v>
@@ -1531,7 +1531,7 @@
         <v>34</v>
       </c>
       <c r="F23">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G23" t="s">
         <v>49</v>
@@ -1566,7 +1566,7 @@
         <v>35</v>
       </c>
       <c r="F24">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G24" t="s">
         <v>49</v>
@@ -1601,7 +1601,7 @@
         <v>36</v>
       </c>
       <c r="F25">
-        <v>96.8</v>
+        <v>94.75</v>
       </c>
       <c r="G25" t="s">
         <v>49</v>
@@ -1636,7 +1636,7 @@
         <v>37</v>
       </c>
       <c r="F26">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G26" t="s">
         <v>49</v>
@@ -1671,7 +1671,7 @@
         <v>38</v>
       </c>
       <c r="F27">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G27" t="s">
         <v>49</v>
@@ -1706,7 +1706,7 @@
         <v>39</v>
       </c>
       <c r="F28">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G28" t="s">
         <v>49</v>
@@ -1741,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="F29">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G29" t="s">
         <v>49</v>
@@ -1776,7 +1776,7 @@
         <v>41</v>
       </c>
       <c r="F30">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G30" t="s">
         <v>49</v>
@@ -1811,7 +1811,7 @@
         <v>42</v>
       </c>
       <c r="F31">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G31" t="s">
         <v>49</v>
@@ -1846,7 +1846,7 @@
         <v>43</v>
       </c>
       <c r="F32">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G32" t="s">
         <v>49</v>
@@ -1881,7 +1881,7 @@
         <v>44</v>
       </c>
       <c r="F33">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G33" t="s">
         <v>49</v>
@@ -1916,7 +1916,7 @@
         <v>45</v>
       </c>
       <c r="F34">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G34" t="s">
         <v>49</v>
@@ -1951,7 +1951,7 @@
         <v>46</v>
       </c>
       <c r="F35">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G35" t="s">
         <v>49</v>
@@ -1986,7 +1986,7 @@
         <v>47</v>
       </c>
       <c r="F36">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G36" t="s">
         <v>49</v>
@@ -2021,7 +2021,7 @@
         <v>48</v>
       </c>
       <c r="F37">
-        <v>112.6</v>
+        <v>107.5</v>
       </c>
       <c r="G37" t="s">
         <v>49</v>

</xml_diff>